<commit_message>
update in training model
</commit_message>
<xml_diff>
--- a/business_cards.xlsx
+++ b/business_cards.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,6 +479,16 @@
           <t>Font Analysis</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>City</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>PIN Code</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -522,6 +532,8 @@
         </is>
       </c>
       <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -565,6 +577,8 @@
         </is>
       </c>
       <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -608,6 +622,8 @@
         </is>
       </c>
       <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -651,6 +667,8 @@
         </is>
       </c>
       <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -694,6 +712,8 @@
         </is>
       </c>
       <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -739,6 +759,175 @@
       <c r="I7" t="inlineStr">
         <is>
           <t>GOPALBHAI +91 84010 18206 (size: 1.24), NAKULBHAI +91 99790 73732 (size: 1.00), RFC (size: 3.61), KULDEVI (size: 10.00), FRUIT COMPAN (size: 3.61)</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>KULDEVI</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>+918401018206, +919979073732</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Bus Stand, Yard Shop, Yard Shop No</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>GOPALBHAI +91 84010 18206 NAKULBHAI +91 99790 73732 RFC KULDEVI FRUIT COMPAN @ld Fruit MMarkket Yard Shop No 57, TRADERS @Opps ! IMPOTER Bus Stand; Gondal 360371.</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>GOPALBHAI +91 84010 18206 NAKULBHAI +91 99790 73732 RFC KULDEVI FRUIT COMPAN @ld Fruit MMarkket Yard Shop No 57, TRADERS @Opps ! IMPOTER Bus Stand; Gondal 360371.</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2025-05-09 15:48:49</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>GOPALBHAI +91 84010 18206 (size: 1.24), NAKULBHAI +91 99790 73732 (size: 1.00), RFC (size: 3.61), KULDEVI (size: 10.00), FRUIT COMPAN (size: 3.61)</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="K8" t="n">
+        <v>360371</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>KULDEVI</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>+918401018206, +919979073732</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Bus Stand, Yard Shop, Yard Shop No</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>GOPALBHAI +91 84010 18206 NAKULBHAI +91 99790 73732 RFC KULDEVI FRUIT COMPAN @ld Fruit MMarkket Yard Shop No 57, TRADERS @Opps ! IMPOTER Bus Stand; Gondal 360371.</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>GOPALBHAI +91 84010 18206 NAKULBHAI +91 99790 73732 RFC KULDEVI FRUIT COMPAN @ld Fruit MMarkket Yard Shop No 57, TRADERS @Opps ! IMPOTER Bus Stand; Gondal 360371.</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2025-05-09 15:48:56</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>GOPALBHAI +91 84010 18206 (size: 1.24), NAKULBHAI +91 99790 73732 (size: 1.00), RFC (size: 3.61), KULDEVI (size: 10.00), FRUIT COMPAN (size: 3.61)</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="K9" t="n">
+        <v>360371</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>KULDEVI</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>+918401018206, +919979073732</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Bus Stand, Yard Shop, Yard Shop No</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>GOPALBHAI +91 84010 18206 NAKULBHAI +91 99790 73732 RFC KULDEVI FRUIT COMPAN @ld Fruit MMarkket Yard Shop No 57, TRADERS @Opps ! IMPOTER Bus Stand; Gondal 360371.</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>GOPALBHAI +91 84010 18206 NAKULBHAI +91 99790 73732 RFC KULDEVI FRUIT COMPAN @ld Fruit MMarkket Yard Shop No 57, TRADERS @Opps ! IMPOTER Bus Stand; Gondal 360371.</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2025-05-13 22:38:09</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>GOPALBHAI +91 84010 18206 (size: 1.24), NAKULBHAI +91 99790 73732 (size: 1.00), RFC (size: 3.61), KULDEVI (size: 10.00), FRUIT COMPAN (size: 3.61)</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>360371</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
InfoCard-AI -> Excel sheet functionallity
</commit_message>
<xml_diff>
--- a/business_cards.xlsx
+++ b/business_cards.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -925,9 +925,121 @@
           <t>Not Found</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>360371</t>
+      <c r="K10" t="n">
+        <v>360371</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>kotak</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>+919409727736</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>L.ranpura@kotak.com</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>L.ranpura, kotak.com, www.kotak.com</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Darshan Ranpura Service</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>360 002, India Main Road</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>kotak Kotak Mahindra Bank Darshan Ranpura Service Officer Assistant Manager Kotak Mahindra Bank Ltd_ D +91281 2812581401 Ground Floor; Chandra Cottage M+91 9409727736 Opp RMC Swimming Pool L.ranpura@kotak.com darshan. Near Kalola Children Hospital, Kothariya www.kotak.com 360 002, India Main Road, Rajkot</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2025-05-15 13:01:31</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>kotak (size: 10.00), Kotak Mahindra Bank (size: 7.85), Darshan Ranpura (size: 4.52), Service Officer (size: 1.59), Assistant Manager (size: 2.96)</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>kotak</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>+919409727736</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>L.ranpura@kotak.com</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>L.ranpura, kotak.com, www.kotak.com</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Darshan Ranpura Service</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>360 002, India Main Road</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>kotak Kotak Mahindra Bank Darshan Ranpura Service Officer Assistant Manager Kotak Mahindra Bank Ltd_ D +91281 2812581401 Ground Floor; Chandra Cottage M+91 9409727736 Opp RMC Swimming Pool L.ranpura@kotak.com darshan. Near Kalola Children Hospital, Kothariya www.kotak.com 360 002, India Main Road, Rajkot</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2025-05-15 13:01:39</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>kotak (size: 10.00), Kotak Mahindra Bank (size: 7.85), Darshan Ranpura (size: 4.52), Service Officer (size: 1.59), Assistant Manager (size: 2.96)</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Not Found</t>
         </is>
       </c>
     </row>

</xml_diff>